<commit_message>
commit: não deixar só na minha maquina
</commit_message>
<xml_diff>
--- a/documentos/dados/Planilha Inteli - dados de rentabilidade.xlsx
+++ b/documentos/dados/Planilha Inteli - dados de rentabilidade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciusmaciel/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E7207F-8086-EF40-ACA7-517D626A4301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA483A4-BBFC-5249-B043-34E2E773C3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6380" yWindow="4620" windowWidth="27820" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Código carteira smart</t>
   </si>
@@ -131,9 +131,6 @@
     <t>Responsável</t>
   </si>
   <si>
-    <t>Estagiário</t>
-  </si>
-  <si>
     <t>Aqui está puxando corretamente</t>
   </si>
   <si>
@@ -143,7 +140,34 @@
     <t>Vinicius Maciel</t>
   </si>
   <si>
-    <t>Vinicius_Maciel_Moderada</t>
+    <t>Helena Miranda</t>
+  </si>
+  <si>
+    <t>Fernandito Banker</t>
+  </si>
+  <si>
+    <t>Renato Banker</t>
+  </si>
+  <si>
+    <t>IPCA + 6%</t>
+  </si>
+  <si>
+    <t>XP INVESTIMENTOS (1.56%)</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>BBB</t>
+  </si>
+  <si>
+    <t>Moderada 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderada 2 </t>
   </si>
 </sst>
 </file>
@@ -507,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -596,13 +620,13 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>11719</v>
+        <v>13317</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -611,7 +635,7 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G2">
         <v>-1.76</v>
@@ -658,10 +682,10 @@
         <v>11421</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -670,7 +694,7 @@
         <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G3">
         <v>0.91</v>
@@ -697,7 +721,7 @@
         <v>28</v>
       </c>
       <c r="O3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P3" t="s">
         <v>30</v>
@@ -706,10 +730,63 @@
         <v>29</v>
       </c>
       <c r="R3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S3" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>13357</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4">
+        <v>1.79</v>
+      </c>
+      <c r="I4">
+        <v>0.63</v>
+      </c>
+      <c r="J4">
+        <v>0.42</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>-0.22</v>
+      </c>
+      <c r="M4">
+        <v>250</v>
+      </c>
+      <c r="N4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -718,6 +795,31 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="ff46ca56-c039-4e9d-bbe3-53481f5c3529">5ZYQRETFUHUN-230250761-234034</_dlc_DocId>
+    <TaxCatchAll xmlns="ff46ca56-c039-4e9d-bbe3-53481f5c3529" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="913bf5ba-6b36-4c8e-bef8-c73438b9f549">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_dlc_DocIdUrl xmlns="ff46ca56-c039-4e9d-bbe3-53481f5c3529">
+      <Url>https://mzrinvestimentos.sharepoint.com/sites/dados/_layouts/15/DocIdRedir.aspx?ID=5ZYQRETFUHUN-230250761-234034</Url>
+      <Description>5ZYQRETFUHUN-230250761-234034</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -765,31 +867,6 @@
     <Filter/>
   </Receiver>
 </spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="ff46ca56-c039-4e9d-bbe3-53481f5c3529">5ZYQRETFUHUN-230250761-234034</_dlc_DocId>
-    <TaxCatchAll xmlns="ff46ca56-c039-4e9d-bbe3-53481f5c3529" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="913bf5ba-6b36-4c8e-bef8-c73438b9f549">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_dlc_DocIdUrl xmlns="ff46ca56-c039-4e9d-bbe3-53481f5c3529">
-      <Url>https://mzrinvestimentos.sharepoint.com/sites/dados/_layouts/15/DocIdRedir.aspx?ID=5ZYQRETFUHUN-230250761-234034</Url>
-      <Description>5ZYQRETFUHUN-230250761-234034</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1073,9 +1150,12 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12C309F5-CBD5-4E48-90C3-22B3BD62C1DE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFF8490-7054-4FE6-93D0-788CBE83641C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ff46ca56-c039-4e9d-bbe3-53481f5c3529"/>
+    <ds:schemaRef ds:uri="913bf5ba-6b36-4c8e-bef8-c73438b9f549"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1089,12 +1169,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFF8490-7054-4FE6-93D0-788CBE83641C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12C309F5-CBD5-4E48-90C3-22B3BD62C1DE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ff46ca56-c039-4e9d-bbe3-53481f5c3529"/>
-    <ds:schemaRef ds:uri="913bf5ba-6b36-4c8e-bef8-c73438b9f549"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
feat: nome do banker puxado corretamente
- implementa a feature do nome do banker ser puxado da coluna "NomePronomeBanker" e adiciona um script que se o banker for o banker 4 (Felipe), o texto só fica com o "Felipe" para evitar duplicação
</commit_message>
<xml_diff>
--- a/documentos/dados/Planilha Inteli - dados de rentabilidade.xlsx
+++ b/documentos/dados/Planilha Inteli - dados de rentabilidade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciusmaciel/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA483A4-BBFC-5249-B043-34E2E773C3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02C1A29-1076-874E-8AA0-0DBF212D48B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6380" yWindow="4620" windowWidth="27820" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,7 +534,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>